<commit_message>
guarding for possible initial value
</commit_message>
<xml_diff>
--- a/customer-review-rules/testsuite.xlsx
+++ b/customer-review-rules/testsuite.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4Work\TechSpecialty\4Giveback\Assets\ODMx\watsonxai-from-odm\customer-review-rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4Work\TechSpecialty\4Giveback\Assets\ODMx\public\watsonxai-from-odm\customer-review-rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8476FC5-7832-49EF-941D-296127B9937B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CD4EA1-3B2B-43C2-9BF7-09C59198B20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23850" yWindow="2100" windowWidth="21390" windowHeight="11475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -663,10 +663,10 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1141,7 +1141,7 @@
   <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -1170,13 +1170,13 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="37" t="s">
+      <c r="E5" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="38" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1238,14 +1238,14 @@
       <c r="C9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="37" t="s">
         <v>50</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>0</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
@@ -1255,14 +1255,14 @@
       <c r="C10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="37" t="s">
         <v>52</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1316,7 +1316,7 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -1384,7 +1384,7 @@
       <c r="B9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -1395,7 +1395,7 @@
       <c r="B10" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="37" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="12" t="s">

</xml_diff>